<commit_message>
email work  for passed tc report
</commit_message>
<xml_diff>
--- a/src/main/resources/testPlan/TestEnvironment.xlsx
+++ b/src/main/resources/testPlan/TestEnvironment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\AMT-TestFrameWork\src\main\resources\testPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A91B28E-58EE-465C-9953-073A405A06F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2402348E-1C6C-4E20-AAB6-59B6CC908EBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>EnvName</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>TCEnv104</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -492,7 +495,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -592,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -621,7 +624,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -650,7 +653,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9">

</xml_diff>